<commit_message>
Neue Funktion: Über die Adminseite kann ab jetzt das Entlassungsdatum eines Patienten verschoben werden. Außerdem wird beim Ändern der Zimmer- und Bettennummer nun auch die Exceltabelle angepasst
</commit_message>
<xml_diff>
--- a/ATOS Projekt/Input/Patienten.xlsx
+++ b/ATOS Projekt/Input/Patienten.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Tabelle1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>Nutzername</t>
   </si>
@@ -31,7 +32,7 @@
     <t>Zimmernummer</t>
   </si>
   <si>
-    <t>Bettennummer</t>
+    <t>Bett</t>
   </si>
   <si>
     <t>Aufnahmedatum</t>
@@ -80,32 +81,46 @@
   </si>
   <si>
     <t>Wosnitza</t>
+  </si>
+  <si>
+    <t>8QZif1</t>
+  </si>
+  <si>
+    <t>pYRG9g3kLa</t>
+  </si>
+  <si>
+    <t>WSTyYx</t>
+  </si>
+  <si>
+    <t>sR3lk4A6Lt</t>
+  </si>
+  <si>
+    <t>gWUjRG</t>
+  </si>
+  <si>
+    <t>wcTS71uby2</t>
+  </si>
+  <si>
+    <t>10.07.2022</t>
+  </si>
+  <si>
+    <t>13.07.2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,59 +131,40 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+  <cellXfs count="7">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" fontId="0" numFmtId="14" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" fontId="0" numFmtId="14" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -177,34 +173,34 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -218,71 +214,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -306,53 +302,54 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -362,7 +359,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -371,7 +368,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -380,7 +377,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -388,10 +385,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -420,7 +417,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -433,12 +430,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -456,27 +454,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="0" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.83203125" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" style="5" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11" customWidth="true" style="4"/>
+    <col min="2" max="2" width="11.5" customWidth="true" style="4"/>
+    <col min="3" max="3" width="12.5" customWidth="true" style="4"/>
+    <col min="4" max="4" width="12.5" customWidth="true" style="4"/>
+    <col min="5" max="5" width="14.6640625" customWidth="true" style="5"/>
+    <col min="6" max="6" width="12.6640625" customWidth="true" style="5"/>
+    <col min="7" max="7" width="15" customWidth="true" style="6"/>
+    <col min="8" max="8" width="16.33203125" customWidth="true" style="6"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:8" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,17 +492,17 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:8" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -519,16 +519,16 @@
         <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3">
         <v>44745</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>44747</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:8" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -542,19 +542,19 @@
         <v>14</v>
       </c>
       <c r="E3" s="2">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>44732</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>44736</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:8" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -568,19 +568,19 @@
         <v>17</v>
       </c>
       <c r="E4" s="2">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>44733</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>44735</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:8" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -597,16 +597,16 @@
         <v>34</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3">
         <v>44727</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>44731</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:8" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -620,19 +620,109 @@
         <v>17</v>
       </c>
       <c r="E6" s="2">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>44735</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>44737</v>
       </c>
     </row>
+    <row r="7" spans="1:8" customHeight="1" ht="17.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>44747</v>
+      </c>
+      <c r="H7" s="3">
+        <v>44749</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5">
+        <v>25</v>
+      </c>
+      <c r="F8" s="5">
+        <v>4</v>
+      </c>
+      <c r="G8" s="6">
+        <v>44749</v>
+      </c>
+      <c r="H8" s="6">
+        <v>44841</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="5">
+        <v>25</v>
+      </c>
+      <c r="F9" s="5">
+        <v>4</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Verbesserung der Darstellung einer Bestellung und Datanbankabfragen aktualisiert
</commit_message>
<xml_diff>
--- a/ATOS Projekt/Input/Patienten.xlsx
+++ b/ATOS Projekt/Input/Patienten.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId4"/>
+    <sheet r:id="rId1" sheetId="1" name="Tabelle1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Nutzername</t>
   </si>
@@ -81,46 +80,26 @@
   </si>
   <si>
     <t>Wosnitza</t>
-  </si>
-  <si>
-    <t>8QZif1</t>
-  </si>
-  <si>
-    <t>pYRG9g3kLa</t>
-  </si>
-  <si>
-    <t>WSTyYx</t>
-  </si>
-  <si>
-    <t>sR3lk4A6Lt</t>
-  </si>
-  <si>
-    <t>gWUjRG</t>
-  </si>
-  <si>
-    <t>wcTS71uby2</t>
-  </si>
-  <si>
-    <t>10.07.2022</t>
-  </si>
-  <si>
-    <t>13.07.2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,40 +110,56 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="14" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="14" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -173,10 +168,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -214,71 +209,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -302,54 +297,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -359,7 +353,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -368,7 +362,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -377,7 +371,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -385,10 +379,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -417,7 +411,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -430,13 +424,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -454,29 +447,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.83203125" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="true" style="4"/>
-    <col min="2" max="2" width="11.5" customWidth="true" style="4"/>
-    <col min="3" max="3" width="12.5" customWidth="true" style="4"/>
-    <col min="4" max="4" width="12.5" customWidth="true" style="4"/>
-    <col min="5" max="5" width="14.6640625" customWidth="true" style="5"/>
-    <col min="6" max="6" width="12.6640625" customWidth="true" style="5"/>
-    <col min="7" max="7" width="15" customWidth="true" style="6"/>
-    <col min="8" max="8" width="16.33203125" customWidth="true" style="6"/>
+    <col min="1" max="1" style="4" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -522,13 +513,13 @@
         <v>4</v>
       </c>
       <c r="G2" s="3">
-        <v>44745</v>
+        <v>44752</v>
       </c>
       <c r="H2" s="3">
-        <v>44747</v>
+        <v>44756</v>
       </c>
     </row>
-    <row r="3" spans="1:8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -554,7 +545,7 @@
         <v>44736</v>
       </c>
     </row>
-    <row r="4" spans="1:8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -580,7 +571,7 @@
         <v>44735</v>
       </c>
     </row>
-    <row r="5" spans="1:8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -600,129 +591,13 @@
         <v>3</v>
       </c>
       <c r="G5" s="3">
-        <v>44727</v>
+        <v>44735</v>
       </c>
       <c r="H5" s="3">
-        <v>44731</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" customHeight="1" ht="17.25">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
-        <v>44735</v>
-      </c>
-      <c r="H6" s="3">
         <v>44737</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" customHeight="1" ht="17.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2">
-        <v>4</v>
-      </c>
-      <c r="G7" s="3">
-        <v>44747</v>
-      </c>
-      <c r="H7" s="3">
-        <v>44749</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5">
-        <v>25</v>
-      </c>
-      <c r="F8" s="5">
-        <v>4</v>
-      </c>
-      <c r="G8" s="6">
-        <v>44749</v>
-      </c>
-      <c r="H8" s="6">
-        <v>44841</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="5">
-        <v>25</v>
-      </c>
-      <c r="F9" s="5">
-        <v>4</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Veränderte Nachricht beim Hilfemodal (Angabe einer Mail Adresse die im Problemfall angeschrieben werden kann und Hinzufügen der Übersetzungsfunktion für jede Seite)
</commit_message>
<xml_diff>
--- a/ATOS Projekt/Input/Patienten.xlsx
+++ b/ATOS Projekt/Input/Patienten.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/ATOS/ATOS Projekt/Input/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC9E516-96E5-D74D-9F3C-0CC2ECA65AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-4960" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Tabelle1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Nutzername</t>
   </si>
@@ -68,6 +74,15 @@
   </si>
   <si>
     <t>Drei</t>
+  </si>
+  <si>
+    <t>Fgk4hj</t>
+  </si>
+  <si>
+    <t>hDfzu85Rf7</t>
+  </si>
+  <si>
+    <t>Vier</t>
   </si>
   <si>
     <t>5djSQb</t>
@@ -85,8 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,7 +111,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -129,35 +143,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -168,10 +194,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -209,71 +235,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -301,7 +327,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -324,11 +350,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -337,13 +363,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -353,7 +379,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -362,7 +388,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -371,7 +397,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -379,10 +405,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -447,27 +473,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="4" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -519,7 +546,7 @@
         <v>44756</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -545,7 +572,7 @@
         <v>44736</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -571,33 +598,60 @@
         <v>44735</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="5">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6">
+        <v>44743</v>
+      </c>
+      <c r="H5" s="6">
+        <v>44746</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2">
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2">
         <v>34</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F6" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G6" s="3">
         <v>44735</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H6" s="3">
         <v>44737</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>